<commit_message>
add most events to oregon trail
</commit_message>
<xml_diff>
--- a/misc/riders calculation.xlsx
+++ b/misc/riders calculation.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="RidersCalc" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="EventsChart" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">if (randomInt(10) &lt;= ((this.totalMileage / 100 - 4) ^ 2 + 72) / ((this.totalMileage / 100 - 4) ^ 2 + 12) - 1) {</t>
   </si>
@@ -36,6 +37,15 @@
   <si>
     <t xml:space="preserve">Quotient</t>
   </si>
+  <si>
+    <t xml:space="preserve">Odds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event Line #</t>
+  </si>
 </sst>
 </file>
 
@@ -49,6 +59,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,7 +125,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -129,6 +140,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -150,7 +165,7 @@
   </sheetPr>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -637,4 +652,216 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3660</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3790</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>3850</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>4130</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>4190</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>4290</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>4610</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>4670</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
oregon: translate mountains code
</commit_message>
<xml_diff>
--- a/misc/riders calculation.xlsx
+++ b/misc/riders calculation.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RidersCalc" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="EventsChart" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="HailStormCalc" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve">if (randomInt(10) &lt;= ((this.totalMileage / 100 - 4) ^ 2 + 72) / ((this.totalMileage / 100 - 4) ^ 2 + 12) - 1) {</t>
   </si>
@@ -45,6 +46,9 @@
   </si>
   <si>
     <t xml:space="preserve">Event Line #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF RND(-1)*10&gt;9-((M/100-15)**2+72)/((M/100-15)**2+12)</t>
   </si>
 </sst>
 </file>
@@ -125,7 +129,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -144,6 +148,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -661,7 +669,7 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -864,4 +872,332 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="19.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>950</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <f aca="false">(A4/100 - 15) ^ 2 + 72</f>
+        <v>102.25</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <f aca="false">(A4/100 -15) ^ 2 + 12</f>
+        <v>42.25</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <f aca="false">B4/C4</f>
+        <v>2.42011834319527</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <f aca="false">A4+100</f>
+        <v>1050</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <f aca="false">(A5/100 - 15) ^ 2 + 72</f>
+        <v>92.25</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <f aca="false">(A5/100 -15) ^ 2 + 12</f>
+        <v>32.25</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <f aca="false">B5/C5</f>
+        <v>2.86046511627907</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <f aca="false">A5+100</f>
+        <v>1150</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <f aca="false">(A6/100 - 15) ^ 2 + 72</f>
+        <v>84.25</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <f aca="false">(A6/100 -15) ^ 2 + 12</f>
+        <v>24.25</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <f aca="false">B6/C6</f>
+        <v>3.47422680412371</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <f aca="false">A6+100</f>
+        <v>1250</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <f aca="false">(A7/100 - 15) ^ 2 + 72</f>
+        <v>78.25</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <f aca="false">(A7/100 -15) ^ 2 + 12</f>
+        <v>18.25</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <f aca="false">B7/C7</f>
+        <v>4.28767123287671</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <f aca="false">A7+100</f>
+        <v>1350</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <f aca="false">(A8/100 - 15) ^ 2 + 72</f>
+        <v>74.25</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <f aca="false">(A8/100 -15) ^ 2 + 12</f>
+        <v>14.25</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <f aca="false">B8/C8</f>
+        <v>5.21052631578947</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <f aca="false">A8+100</f>
+        <v>1450</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <f aca="false">(A9/100 - 15) ^ 2 + 72</f>
+        <v>72.25</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <f aca="false">(A9/100 -15) ^ 2 + 12</f>
+        <v>12.25</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <f aca="false">B9/C9</f>
+        <v>5.89795918367347</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <f aca="false">A9+100</f>
+        <v>1550</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <f aca="false">(A10/100 - 15) ^ 2 + 72</f>
+        <v>72.25</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <f aca="false">(A10/100 -15) ^ 2 + 12</f>
+        <v>12.25</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <f aca="false">B10/C10</f>
+        <v>5.89795918367347</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <f aca="false">A10+100</f>
+        <v>1650</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <f aca="false">(A11/100 - 15) ^ 2 + 72</f>
+        <v>74.25</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <f aca="false">(A11/100 -15) ^ 2 + 12</f>
+        <v>14.25</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <f aca="false">B11/C11</f>
+        <v>5.21052631578947</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <f aca="false">A11+100</f>
+        <v>1750</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <f aca="false">(A12/100 - 15) ^ 2 + 72</f>
+        <v>78.25</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <f aca="false">(A12/100 -15) ^ 2 + 12</f>
+        <v>18.25</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <f aca="false">B12/C12</f>
+        <v>4.28767123287671</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <f aca="false">A12+100</f>
+        <v>1850</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <f aca="false">(A13/100 - 15) ^ 2 + 72</f>
+        <v>84.25</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <f aca="false">(A13/100 -15) ^ 2 + 12</f>
+        <v>24.25</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <f aca="false">B13/C13</f>
+        <v>3.47422680412371</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <f aca="false">A13+100</f>
+        <v>1950</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <f aca="false">(A14/100 - 15) ^ 2 + 72</f>
+        <v>92.25</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <f aca="false">(A14/100 -15) ^ 2 + 12</f>
+        <v>32.25</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <f aca="false">B14/C14</f>
+        <v>2.86046511627907</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <f aca="false">A14+100</f>
+        <v>2050</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <f aca="false">(A15/100 - 15) ^ 2 + 72</f>
+        <v>102.25</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <f aca="false">(A15/100 -15) ^ 2 + 12</f>
+        <v>42.25</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <f aca="false">B15/C15</f>
+        <v>2.42011834319527</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix arithmetic operator misuse
</commit_message>
<xml_diff>
--- a/misc/riders calculation.xlsx
+++ b/misc/riders calculation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t xml:space="preserve">if (randomInt(10) &lt;= ((this.totalMileage / 100 - 4) ^ 2 + 72) / ((this.totalMileage / 100 - 4) ^ 2 + 12) - 1) {</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t xml:space="preserve">IF RND(-1)*10&gt;9-((M/100-15)**2+72)/((M/100-15)**2+12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NineMinus</t>
   </si>
 </sst>
 </file>
@@ -879,10 +882,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -910,6 +913,9 @@
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
@@ -926,6 +932,10 @@
       <c r="D4" s="3" t="n">
         <f aca="false">B4/C4</f>
         <v>2.42011834319527</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">9-D4</f>
+        <v>6.57988165680473</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -945,6 +955,10 @@
         <f aca="false">B5/C5</f>
         <v>2.86046511627907</v>
       </c>
+      <c r="E5" s="1" t="n">
+        <f aca="false">9-D5</f>
+        <v>6.13953488372093</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -963,10 +977,13 @@
         <f aca="false">B6/C6</f>
         <v>3.47422680412371</v>
       </c>
+      <c r="E6" s="1" t="n">
+        <f aca="false">9-D6</f>
+        <v>5.52577319587629</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <f aca="false">A6+100</f>
         <v>1250</v>
       </c>
       <c r="B7" s="3" t="n">
@@ -980,6 +997,10 @@
       <c r="D7" s="3" t="n">
         <f aca="false">B7/C7</f>
         <v>4.28767123287671</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <f aca="false">9-D7</f>
+        <v>4.71232876712329</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,6 +1020,10 @@
         <f aca="false">B8/C8</f>
         <v>5.21052631578947</v>
       </c>
+      <c r="E8" s="1" t="n">
+        <f aca="false">9-D8</f>
+        <v>3.78947368421053</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -1017,6 +1042,10 @@
         <f aca="false">B9/C9</f>
         <v>5.89795918367347</v>
       </c>
+      <c r="E9" s="1" t="n">
+        <f aca="false">9-D9</f>
+        <v>3.10204081632653</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -1035,6 +1064,10 @@
         <f aca="false">B10/C10</f>
         <v>5.89795918367347</v>
       </c>
+      <c r="E10" s="1" t="n">
+        <f aca="false">9-D10</f>
+        <v>3.10204081632653</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -1053,6 +1086,10 @@
         <f aca="false">B11/C11</f>
         <v>5.21052631578947</v>
       </c>
+      <c r="E11" s="1" t="n">
+        <f aca="false">9-D11</f>
+        <v>3.78947368421053</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -1071,6 +1108,10 @@
         <f aca="false">B12/C12</f>
         <v>4.28767123287671</v>
       </c>
+      <c r="E12" s="1" t="n">
+        <f aca="false">9-D12</f>
+        <v>4.71232876712329</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -1089,6 +1130,10 @@
         <f aca="false">B13/C13</f>
         <v>3.47422680412371</v>
       </c>
+      <c r="E13" s="1" t="n">
+        <f aca="false">9-D13</f>
+        <v>5.52577319587629</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -1107,6 +1152,10 @@
         <f aca="false">B14/C14</f>
         <v>2.86046511627907</v>
       </c>
+      <c r="E14" s="1" t="n">
+        <f aca="false">9-D14</f>
+        <v>6.13953488372093</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -1125,46 +1174,186 @@
         <f aca="false">B15/C15</f>
         <v>2.42011834319527</v>
       </c>
+      <c r="E15" s="1" t="n">
+        <f aca="false">9-D15</f>
+        <v>6.57988165680473</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="A16" s="1" t="n">
+        <f aca="false">A15+100</f>
+        <v>2150</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <f aca="false">(A16/100 - 15) ^ 2 + 72</f>
+        <v>114.25</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <f aca="false">(A16/100 -15) ^ 2 + 12</f>
+        <v>54.25</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <f aca="false">B16/C16</f>
+        <v>2.10599078341014</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <f aca="false">9-D16</f>
+        <v>6.89400921658986</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="1" t="n">
+        <f aca="false">A16+100</f>
+        <v>2250</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <f aca="false">(A17/100 - 15) ^ 2 + 72</f>
+        <v>128.25</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <f aca="false">(A17/100 -15) ^ 2 + 12</f>
+        <v>68.25</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <f aca="false">B17/C17</f>
+        <v>1.87912087912088</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <f aca="false">9-D17</f>
+        <v>7.12087912087912</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="1" t="n">
+        <f aca="false">A17+100</f>
+        <v>2350</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <f aca="false">(A18/100 - 15) ^ 2 + 72</f>
+        <v>144.25</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <f aca="false">(A18/100 -15) ^ 2 + 12</f>
+        <v>84.25</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <f aca="false">B18/C18</f>
+        <v>1.71216617210682</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <f aca="false">9-D18</f>
+        <v>7.28783382789318</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="1" t="n">
+        <f aca="false">A18+100</f>
+        <v>2450</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <f aca="false">(A19/100 - 15) ^ 2 + 72</f>
+        <v>162.25</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <f aca="false">(A19/100 -15) ^ 2 + 12</f>
+        <v>102.25</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <f aca="false">B19/C19</f>
+        <v>1.58679706601467</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <f aca="false">9-D19</f>
+        <v>7.41320293398533</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="1" t="n">
+        <f aca="false">A19+100</f>
+        <v>2550</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <f aca="false">(A20/100 - 15) ^ 2 + 72</f>
+        <v>182.25</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <f aca="false">(A20/100 -15) ^ 2 + 12</f>
+        <v>122.25</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <f aca="false">B20/C20</f>
+        <v>1.49079754601227</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <f aca="false">9-D20</f>
+        <v>7.50920245398773</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="1" t="n">
+        <f aca="false">A20+100</f>
+        <v>2650</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <f aca="false">(A21/100 - 15) ^ 2 + 72</f>
+        <v>204.25</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <f aca="false">(A21/100 -15) ^ 2 + 12</f>
+        <v>144.25</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <f aca="false">B21/C21</f>
+        <v>1.4159445407279</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <f aca="false">9-D21</f>
+        <v>7.5840554592721</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="1" t="n">
+        <f aca="false">A21+100</f>
+        <v>2750</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <f aca="false">(A22/100 - 15) ^ 2 + 72</f>
+        <v>228.25</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <f aca="false">(A22/100 -15) ^ 2 + 12</f>
+        <v>168.25</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <f aca="false">B22/C22</f>
+        <v>1.35661218424963</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <f aca="false">9-D22</f>
+        <v>7.64338781575037</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="1" t="n">
+        <f aca="false">A22+100</f>
+        <v>2850</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <f aca="false">(A23/100 - 15) ^ 2 + 72</f>
+        <v>254.25</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <f aca="false">(A23/100 -15) ^ 2 + 12</f>
+        <v>194.25</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <f aca="false">B23/C23</f>
+        <v>1.30888030888031</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <f aca="false">9-D23</f>
+        <v>7.69111969111969</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3"/>

</xml_diff>